<commit_message>
updates to subset TTL file
</commit_message>
<xml_diff>
--- a/doc/MedDRA-3Patient-Subsetting.xlsx
+++ b/doc/MedDRA-3Patient-Subsetting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\MedDRAasRDF\r\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\MedDRAasRDF\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E47C8B-4E32-4BA8-8779-B379CA3A7E37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F272F1-389F-42B1-AE48-5FA2E471BD4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,7 +569,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -704,77 +704,77 @@
       <c r="A8" s="9">
         <v>1015</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="11">
-        <v>10003058</v>
-      </c>
-      <c r="D8" s="11">
-        <v>10003041</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="B8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="10">
+        <v>10003047</v>
+      </c>
+      <c r="D8" s="10">
+        <v>10003053</v>
+      </c>
+      <c r="E8" s="10">
         <v>10003057</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>10001316</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="10">
         <v>10018065</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
-        <v>1015</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="11">
-        <v>10003058</v>
-      </c>
-      <c r="D9" s="11">
-        <v>10003041</v>
-      </c>
-      <c r="E9" s="12">
+        <v>1028</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10">
+        <v>10003047</v>
+      </c>
+      <c r="D9" s="10">
+        <v>10003053</v>
+      </c>
+      <c r="E9" s="10">
         <v>10003057</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
         <v>10001316</v>
       </c>
-      <c r="G9" s="13">
-        <v>10022117</v>
+      <c r="G9" s="10">
+        <v>10018065</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>1015</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="11">
-        <v>10003058</v>
-      </c>
-      <c r="D10" s="11">
-        <v>10003041</v>
-      </c>
-      <c r="E10" s="14">
-        <v>10015151</v>
-      </c>
-      <c r="F10" s="14">
-        <v>10014982</v>
-      </c>
-      <c r="G10" s="13">
-        <v>10040785</v>
+      <c r="B10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="10">
+        <v>10003047</v>
+      </c>
+      <c r="D10" s="10">
+        <v>10003053</v>
+      </c>
+      <c r="E10" s="10">
+        <v>10003057</v>
+      </c>
+      <c r="F10" s="10">
+        <v>10001316</v>
+      </c>
+      <c r="G10" s="10">
+        <v>10022117</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
-        <v>1015</v>
+        <v>1028</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C11" s="10">
         <v>10003047</v>
@@ -789,7 +789,7 @@
         <v>10001316</v>
       </c>
       <c r="G11" s="10">
-        <v>10018065</v>
+        <v>10022117</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -806,21 +806,21 @@
         <v>10003053</v>
       </c>
       <c r="E12" s="10">
-        <v>10003057</v>
+        <v>10049293</v>
       </c>
       <c r="F12" s="10">
-        <v>10001316</v>
+        <v>10014982</v>
       </c>
       <c r="G12" s="10">
-        <v>10022117</v>
+        <v>10040785</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
-        <v>1015</v>
+        <v>1028</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C13" s="10">
         <v>10003047</v>
@@ -840,70 +840,70 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
-        <v>1028</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="10">
-        <v>10003047</v>
-      </c>
-      <c r="D14" s="10">
-        <v>10003053</v>
-      </c>
-      <c r="E14" s="10">
+        <v>1015</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="11">
+        <v>10003058</v>
+      </c>
+      <c r="D14" s="11">
+        <v>10003041</v>
+      </c>
+      <c r="E14" s="12">
         <v>10003057</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="12">
         <v>10001316</v>
       </c>
-      <c r="G14" s="10">
-        <v>10022117</v>
+      <c r="G14" s="13">
+        <v>10018065</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
-        <v>1028</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="10">
-        <v>10003047</v>
-      </c>
-      <c r="D15" s="10">
-        <v>10003053</v>
-      </c>
-      <c r="E15" s="10">
+        <v>1015</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="11">
+        <v>10003058</v>
+      </c>
+      <c r="D15" s="11">
+        <v>10003041</v>
+      </c>
+      <c r="E15" s="12">
         <v>10003057</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="12">
         <v>10001316</v>
       </c>
-      <c r="G15" s="10">
-        <v>10018065</v>
+      <c r="G15" s="13">
+        <v>10022117</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
-        <v>1028</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="10">
-        <v>10003047</v>
-      </c>
-      <c r="D16" s="10">
-        <v>10003053</v>
-      </c>
-      <c r="E16" s="10">
-        <v>10049293</v>
-      </c>
-      <c r="F16" s="10">
+        <v>1015</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="11">
+        <v>10003058</v>
+      </c>
+      <c r="D16" s="11">
+        <v>10003041</v>
+      </c>
+      <c r="E16" s="14">
+        <v>10015151</v>
+      </c>
+      <c r="F16" s="14">
         <v>10014982</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="13">
         <v>10040785</v>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C23" s="7">
         <f>SUMPRODUCT(1/COUNTIF(C5:C22,C5:C22&amp;""))</f>
-        <v>6.9999999999999991</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="D23" s="7">
         <f>SUMPRODUCT(1/COUNTIF(D5:D22,D5:D22&amp;""))</f>
@@ -1102,7 +1102,7 @@
     </row>
   </sheetData>
   <sortState ref="A5:G22">
-    <sortCondition ref="D5:D22"/>
+    <sortCondition ref="C5:C22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>